<commit_message>
Updates to latest US develop branch
</commit_message>
<xml_diff>
--- a/InputData/ccs/BCS/BAU CCS Subsidy.xlsx
+++ b/InputData/ccs/BCS/BAU CCS Subsidy.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\Kentucky\eps-kentucky\InputData\ccs\BCS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\ccs\BCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4980F67B-0D0E-4942-ABFD-8FB5DFE0CDE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F268FE25-6FA1-4964-97BE-7705BD55074C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="Electricity Calculations" sheetId="5" r:id="rId2"/>
-    <sheet name="BCS" sheetId="4" r:id="rId3"/>
+    <sheet name="BCS-BCS" sheetId="4" r:id="rId3"/>
+    <sheet name="BCS-DoSfCS" sheetId="6" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="solver_adj" localSheetId="0" hidden="1">About!$A$11</definedName>
@@ -61,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Source:</t>
   </si>
@@ -106,6 +107,18 @@
   </si>
   <si>
     <t>For electricity, adjust the credit value based on its duration relative to the financing repayment period</t>
+  </si>
+  <si>
+    <t>Years</t>
+  </si>
+  <si>
+    <t>Duration</t>
+  </si>
+  <si>
+    <t>45Q Duration</t>
+  </si>
+  <si>
+    <t>12 years</t>
   </si>
 </sst>
 </file>
@@ -161,7 +174,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -172,7 +185,6 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -479,25 +491,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.28515625" customWidth="1"/>
-    <col min="2" max="2" width="55.85546875" customWidth="1"/>
-    <col min="4" max="4" width="30.5703125" customWidth="1"/>
+    <col min="1" max="1" width="30.33203125" customWidth="1"/>
+    <col min="2" max="2" width="55.88671875" customWidth="1"/>
+    <col min="4" max="4" width="30.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -505,22 +517,22 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>0.78500000000000003</v>
       </c>
@@ -528,12 +540,20 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="6">
         <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -550,12 +570,12 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -564,7 +584,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -572,7 +592,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -580,7 +600,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -601,17 +621,17 @@
   </sheetPr>
   <dimension ref="A1:AE3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2:M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" customWidth="1"/>
+    <col min="1" max="1" width="19.44140625" customWidth="1"/>
+    <col min="2" max="2" width="24.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -706,7 +726,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:31" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -716,45 +736,45 @@
       <c r="C2" s="4">
         <v>0</v>
       </c>
-      <c r="D2" s="8">
-        <f>'Electricity Calculations'!$B$4*About!$A$9</f>
-        <v>40.035000000000004</v>
-      </c>
-      <c r="E2" s="8">
-        <f>'Electricity Calculations'!$B$4*About!$A$9</f>
-        <v>40.035000000000004</v>
-      </c>
-      <c r="F2" s="8">
-        <f>'Electricity Calculations'!$B$4*About!$A$9</f>
-        <v>40.035000000000004</v>
-      </c>
-      <c r="G2" s="8">
-        <f>'Electricity Calculations'!$B$4*About!$A$9</f>
-        <v>40.035000000000004</v>
-      </c>
-      <c r="H2" s="8">
-        <f>'Electricity Calculations'!$B$4*About!$A$9</f>
-        <v>40.035000000000004</v>
-      </c>
-      <c r="I2" s="8">
-        <f>'Electricity Calculations'!$B$4*About!$A$9</f>
-        <v>40.035000000000004</v>
-      </c>
-      <c r="J2" s="8">
-        <f>'Electricity Calculations'!$B$4*About!$A$9</f>
-        <v>40.035000000000004</v>
-      </c>
-      <c r="K2" s="8">
-        <f>'Electricity Calculations'!$B$4*About!$A$9</f>
-        <v>40.035000000000004</v>
-      </c>
-      <c r="L2" s="8">
-        <f>'Electricity Calculations'!$B$4*About!$A$9</f>
-        <v>40.035000000000004</v>
-      </c>
-      <c r="M2" s="8">
-        <f>'Electricity Calculations'!$B$4*About!$A$9</f>
-        <v>40.035000000000004</v>
+      <c r="D2">
+        <f>About!$B$11*About!$A$9</f>
+        <v>66.725000000000009</v>
+      </c>
+      <c r="E2">
+        <f>About!$B$11*About!$A$9</f>
+        <v>66.725000000000009</v>
+      </c>
+      <c r="F2">
+        <f>About!$B$11*About!$A$9</f>
+        <v>66.725000000000009</v>
+      </c>
+      <c r="G2">
+        <f>About!$B$11*About!$A$9</f>
+        <v>66.725000000000009</v>
+      </c>
+      <c r="H2">
+        <f>About!$B$11*About!$A$9</f>
+        <v>66.725000000000009</v>
+      </c>
+      <c r="I2">
+        <f>About!$B$11*About!$A$9</f>
+        <v>66.725000000000009</v>
+      </c>
+      <c r="J2">
+        <f>About!$B$11*About!$A$9</f>
+        <v>66.725000000000009</v>
+      </c>
+      <c r="K2">
+        <f>About!$B$11*About!$A$9</f>
+        <v>66.725000000000009</v>
+      </c>
+      <c r="L2">
+        <f>About!$B$11*About!$A$9</f>
+        <v>66.725000000000009</v>
+      </c>
+      <c r="M2">
+        <f>About!$B$11*About!$A$9</f>
+        <v>66.725000000000009</v>
       </c>
       <c r="N2">
         <v>0</v>
@@ -811,7 +831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:31" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -914,6 +934,243 @@
       </c>
       <c r="AE3">
         <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5698252-CD29-4D86-9D7F-2214C5598602}">
+  <sheetPr>
+    <tabColor theme="3"/>
+  </sheetPr>
+  <dimension ref="A1:AE2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1">
+        <v>2021</v>
+      </c>
+      <c r="C1">
+        <v>2022</v>
+      </c>
+      <c r="D1">
+        <v>2023</v>
+      </c>
+      <c r="E1">
+        <v>2024</v>
+      </c>
+      <c r="F1">
+        <v>2025</v>
+      </c>
+      <c r="G1">
+        <v>2026</v>
+      </c>
+      <c r="H1">
+        <v>2027</v>
+      </c>
+      <c r="I1">
+        <v>2028</v>
+      </c>
+      <c r="J1">
+        <v>2029</v>
+      </c>
+      <c r="K1">
+        <v>2030</v>
+      </c>
+      <c r="L1">
+        <v>2031</v>
+      </c>
+      <c r="M1">
+        <v>2032</v>
+      </c>
+      <c r="N1">
+        <v>2033</v>
+      </c>
+      <c r="O1">
+        <v>2034</v>
+      </c>
+      <c r="P1">
+        <v>2035</v>
+      </c>
+      <c r="Q1">
+        <v>2036</v>
+      </c>
+      <c r="R1">
+        <v>2037</v>
+      </c>
+      <c r="S1">
+        <v>2038</v>
+      </c>
+      <c r="T1">
+        <v>2039</v>
+      </c>
+      <c r="U1">
+        <v>2040</v>
+      </c>
+      <c r="V1">
+        <v>2041</v>
+      </c>
+      <c r="W1">
+        <v>2042</v>
+      </c>
+      <c r="X1">
+        <v>2043</v>
+      </c>
+      <c r="Y1">
+        <v>2044</v>
+      </c>
+      <c r="Z1">
+        <v>2045</v>
+      </c>
+      <c r="AA1">
+        <v>2046</v>
+      </c>
+      <c r="AB1">
+        <v>2047</v>
+      </c>
+      <c r="AC1">
+        <v>2048</v>
+      </c>
+      <c r="AD1">
+        <v>2049</v>
+      </c>
+      <c r="AE1">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2">
+        <v>12</v>
+      </c>
+      <c r="C2">
+        <f>$B$2</f>
+        <v>12</v>
+      </c>
+      <c r="D2">
+        <f>$B$2</f>
+        <v>12</v>
+      </c>
+      <c r="E2">
+        <f t="shared" ref="E2:AE2" si="0">$B$2</f>
+        <v>12</v>
+      </c>
+      <c r="F2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="G2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="H2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="I2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="J2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="K2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="L2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="M2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="N2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="O2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="P2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="Q2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="R2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="S2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="T2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="U2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="V2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="W2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="X2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="Y2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="Z2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="AA2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="AB2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="AC2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="AD2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="AE2">
+        <f t="shared" si="0"/>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>